<commit_message>
villarael was the one ruining it
</commit_message>
<xml_diff>
--- a/laliga2223raw.xlsx
+++ b/laliga2223raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.ucl.ac.uk\homee\zcakihe\Documents\18aprilDissertationOfficialMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97061D41-6EDC-4783-B746-7B7D2AAE97E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBFE64F-29E8-4654-98D2-BB43DC28E593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9750" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="105">
   <si>
     <t>Wk</t>
   </si>
@@ -342,9 +342,6 @@
   </si>
   <si>
     <t>Antonio Matéu</t>
-  </si>
-  <si>
-    <t>Estadio de la Cerámica</t>
   </si>
   <si>
     <t>3–4</t>
@@ -1247,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D337" sqref="D337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7728,7 +7725,7 @@
         <v>21088</v>
       </c>
       <c r="K154" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L154" s="3" t="s">
         <v>76</v>
@@ -8610,7 +8607,7 @@
         <v>15129</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L175" s="3" t="s">
         <v>18</v>
@@ -9198,7 +9195,7 @@
         <v>14378</v>
       </c>
       <c r="K189" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L189" s="3" t="s">
         <v>69</v>
@@ -9480,7 +9477,7 @@
         <v>3.4</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H196" s="3">
         <v>1.9</v>
@@ -10038,7 +10035,7 @@
         <v>21178</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L209" s="3" t="s">
         <v>34</v>
@@ -10152,7 +10149,7 @@
         <v>3</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H212" s="3">
         <v>1.8</v>
@@ -10278,7 +10275,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H215" s="3">
         <v>1.2</v>
@@ -10846,7 +10843,7 @@
       </c>
       <c r="J231" s="6"/>
       <c r="K231" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L231" s="3"/>
       <c r="M231" s="3"/>
@@ -11386,7 +11383,7 @@
       </c>
       <c r="J249" s="6"/>
       <c r="K249" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L249" s="3"/>
       <c r="M249" s="3"/>
@@ -11986,7 +11983,7 @@
       </c>
       <c r="J269" s="6"/>
       <c r="K269" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L269" s="3"/>
       <c r="M269" s="3"/>
@@ -12406,7 +12403,7 @@
       </c>
       <c r="J283" s="6"/>
       <c r="K283" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L283" s="3"/>
       <c r="M283" s="3"/>
@@ -13216,7 +13213,7 @@
       </c>
       <c r="J310" s="2"/>
       <c r="K310" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L310" s="2"/>
       <c r="M310" s="3"/>
@@ -13426,7 +13423,7 @@
       </c>
       <c r="J317" s="2"/>
       <c r="K317" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L317" s="2"/>
       <c r="M317" s="3"/>
@@ -14126,7 +14123,7 @@
       </c>
       <c r="J341" s="2"/>
       <c r="K341" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L341" s="2"/>
       <c r="M341" s="3"/>
@@ -14686,7 +14683,7 @@
       </c>
       <c r="J361" s="2"/>
       <c r="K361" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L361" s="2"/>
       <c r="M361" s="3"/>
@@ -15246,7 +15243,7 @@
       </c>
       <c r="J381" s="2"/>
       <c r="K381" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L381" s="2"/>
       <c r="M381" s="3"/>

</xml_diff>